<commit_message>
gráficas y vars en matriz
</commit_message>
<xml_diff>
--- a/matriz de consistencia.xlsx
+++ b/matriz de consistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://econometriasa-my.sharepoint.com/personal/marias_econometria_com/Documents/Github Desktop/FIS/Procesamiento3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{83B3DD0A-5429-43C2-A039-F1F308FA4603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2184054D-265D-4941-BA3D-50B4F99D4B21}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{83B3DD0A-5429-43C2-A039-F1F308FA4603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF96214E-6F83-4F4A-A28C-C6B93AEC09F0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{05460EC6-EDA1-4B90-8C09-A02B89EE68D2}"/>
   </bookViews>
@@ -841,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09899699-F5F6-49B7-A69E-FDA70DAD2F23}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,7 @@
         <v>11</v>
       </c>
       <c r="G18">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
@@ -1358,6 +1358,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="E25:E27"/>
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
@@ -1367,13 +1374,6 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="F3:F7"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="E25:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>